<commit_message>
began logic for passing tests, adjacency is in the works. copied and changed stuff for cluePaths assignment..... have not started targets, reference from clue paths is commented out in bottom
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Desktop\Desktop\School\Mines\Fall2014\SoftwareEng\Clue\clueBoard\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="12435" windowHeight="9525"/>
+    <workbookView xWindow="480" yWindow="140" windowWidth="21780" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -302,7 +302,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -337,7 +337,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,13 +548,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -758,7 +758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -826,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -894,7 +894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -962,7 +962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
@@ -2526,109 +2526,117 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
+      <c r="A30">
+        <v>0</v>
+      </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I30">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K30">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L30">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M30">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N30">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O30">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P30">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q30">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R30">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S30">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T30">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U30">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
       <c r="B33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6">
       <c r="B34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6">
       <c r="B35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6">
       <c r="B36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6">
       <c r="B37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6">
       <c r="B38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6">
       <c r="B39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6">
       <c r="F42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2638,9 +2646,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2650,8 +2663,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all adjacency tests passed, added edge of board tests, and updated xcel clue board layout
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="140" windowWidth="21780" windowHeight="13680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="31">
   <si>
     <t>X</t>
   </si>
@@ -111,13 +111,16 @@
   </si>
   <si>
     <t>Number of doors:  18</t>
+  </si>
+  <si>
+    <t>Light Red: edge of board adjacency tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +135,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +213,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -204,10 +229,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,8 +272,21 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,16 +594,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -615,7 +663,7 @@
       <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="11" t="s">
         <v>8</v>
       </c>
       <c r="V1">
@@ -1839,7 +1887,7 @@
       <c r="T19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="U19" s="9" t="s">
         <v>2</v>
       </c>
       <c r="V19">
@@ -2459,7 +2507,7 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2519,7 +2567,7 @@
       <c r="T29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="U29" s="11" t="s">
         <v>2</v>
       </c>
       <c r="V29">
@@ -2603,31 +2651,36 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
-      <c r="F42" s="8"/>
+    <row r="43" spans="2:6">
+      <c r="F43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tests written for computer targets
</commit_message>
<xml_diff>
--- a/ClueBoardLayout.xlsx
+++ b/ClueBoardLayout.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="13680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14355" windowHeight="13680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,13 +596,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -806,7 +806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -874,7 +874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1690,8 +1690,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1758,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>13</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2639,47 +2639,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F43" s="8"/>
     </row>
   </sheetData>
@@ -2699,7 +2699,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2716,7 +2716,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>